<commit_message>
Added more gold truth for a single company
</commit_message>
<xml_diff>
--- a/manual_download/Amt für Statistik Berlin-Brandenburg/AP_Geschaeftsbericht_DE_2020_BBB.xlsx
+++ b/manual_download/Amt für Statistik Berlin-Brandenburg/AP_Geschaeftsbericht_DE_2020_BBB.xlsx
@@ -19,30 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author>Unknown Author</author>
-  </authors>
-  <commentList>
-    <comment ref="C23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Forderungen gegen Trägerländer</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="42">
   <si>
     <t xml:space="preserve">E1</t>
   </si>
@@ -144,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">Forderungen gegen Unternehmen, mit denen ein Beteiligungsverhaeltnis besteht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forderungen gegen Traegerlaender</t>
   </si>
   <si>
     <t xml:space="preserve">Sonstige Vermoegensgegenstaende</t>
@@ -174,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -195,11 +176,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -398,10 +374,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -480,7 +456,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>10949</v>
+        <v>109490</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>187739</v>
@@ -697,49 +673,49 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="4" t="s">
+    <row r="23" s="2" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="5" t="n">
+    </row>
+    <row r="24" s="5" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E23" s="5" t="n">
+      <c r="E24" s="5" t="n">
         <v>529263.75</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="2" t="n">
+      <c r="C25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2" t="n">
         <v>157007.53</v>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E25" s="2" t="n">
         <v>305557.51</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,45 +723,56 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="2" t="n">
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="2" t="n">
         <v>10489023.37</v>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E28" s="2" t="n">
         <v>6440570.09</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>443040.2</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>338564.1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="2" t="n">
+        <v>443040.2</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>338564.1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -796,6 +783,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>